<commit_message>
Updated rubric to have value per task
</commit_message>
<xml_diff>
--- a/GroupProject/SuperCoolFunYay Rubric.xlsx
+++ b/GroupProject/SuperCoolFunYay Rubric.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hedley\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hedley\Desktop\RTA_SuperCoolFunYay\GroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>SuperCoolFunYay</t>
   </si>
@@ -61,12 +61,21 @@
   <si>
     <t>Render the mesh onto bones</t>
   </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Worth</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -97,13 +106,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -113,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -121,11 +123,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -134,9 +145,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1004"/>
+  <dimension ref="A1:AA1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -466,7 +490,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
@@ -619,10 +643,9 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -650,13 +673,16 @@
       <c r="AA6" s="2"/>
     </row>
     <row r="7" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
+      <c r="A7" s="10" t="s">
+        <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>5</v>
+      <c r="B7" s="11" t="s">
+        <v>14</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -682,14 +708,15 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>10</v>
+      <c r="A8" s="8" t="s">
+        <v>9</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>6</v>
+      <c r="B8" s="8" t="s">
+        <v>5</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C8" s="8">
+        <v>30</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -714,15 +741,17 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
     </row>
-    <row r="9" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
+    <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>10</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
+      <c r="B9" s="8" t="s">
+        <v>6</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="9">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -747,15 +776,17 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
+    <row r="10" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
+      <c r="B10" s="9" t="s">
+        <v>8</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="9">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -781,10 +812,16 @@
       <c r="AA10" s="2"/>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="9">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -809,11 +846,11 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -838,10 +875,10 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -868,10 +905,10 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -984,7 +1021,7 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1013,7 +1050,7 @@
       <c r="AA18" s="2"/>
     </row>
     <row r="19" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1099,8 +1136,8 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+    <row r="22" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1128,11 +1165,11 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1158,10 +1195,10 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1187,10 +1224,10 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1332,7 +1369,7 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
+      <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1361,7 +1398,7 @@
       <c r="AA30" s="2"/>
     </row>
     <row r="31" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
+      <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1447,8 +1484,8 @@
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
+    <row r="34" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1476,11 +1513,11 @@
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
     </row>
-    <row r="35" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -1506,10 +1543,10 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1535,10 +1572,10 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -1680,7 +1717,7 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
+      <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1709,7 +1746,7 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
+      <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -29606,6 +29643,35 @@
       <c r="Z1004" s="2"/>
       <c r="AA1004" s="2"/>
     </row>
+    <row r="1005" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1005" s="2"/>
+      <c r="B1005" s="2"/>
+      <c r="C1005" s="2"/>
+      <c r="D1005" s="2"/>
+      <c r="E1005" s="2"/>
+      <c r="F1005" s="2"/>
+      <c r="G1005" s="2"/>
+      <c r="H1005" s="2"/>
+      <c r="I1005" s="2"/>
+      <c r="J1005" s="2"/>
+      <c r="K1005" s="2"/>
+      <c r="L1005" s="2"/>
+      <c r="M1005" s="2"/>
+      <c r="N1005" s="2"/>
+      <c r="O1005" s="2"/>
+      <c r="P1005" s="2"/>
+      <c r="Q1005" s="2"/>
+      <c r="R1005" s="2"/>
+      <c r="S1005" s="2"/>
+      <c r="T1005" s="2"/>
+      <c r="U1005" s="2"/>
+      <c r="V1005" s="2"/>
+      <c r="W1005" s="2"/>
+      <c r="X1005" s="2"/>
+      <c r="Y1005" s="2"/>
+      <c r="Z1005" s="2"/>
+      <c r="AA1005" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Final Update to Rubric
</commit_message>
<xml_diff>
--- a/GroupProject/SuperCoolFunYay Rubric.xlsx
+++ b/GroupProject/SuperCoolFunYay Rubric.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>SuperCoolFunYay</t>
   </si>
@@ -38,30 +38,6 @@
     <t>Justin Parks</t>
   </si>
   <si>
-    <t>Convert mesh data from FBX to a binary file format</t>
-  </si>
-  <si>
-    <t>Load data from the binary file</t>
-  </si>
-  <si>
-    <t>Render Bones</t>
-  </si>
-  <si>
-    <t>Render the bones in a bind position</t>
-  </si>
-  <si>
-    <t>FBX to Binary</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
-    <t>Render Mesh</t>
-  </si>
-  <si>
-    <t>Render the mesh onto bones</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
@@ -69,6 +45,36 @@
   </si>
   <si>
     <t>Worth</t>
+  </si>
+  <si>
+    <t>Setup Project</t>
+  </si>
+  <si>
+    <t>Load and Render</t>
+  </si>
+  <si>
+    <t>Load and render from FBX</t>
+  </si>
+  <si>
+    <t>Setup base project with structures</t>
+  </si>
+  <si>
+    <t>Setup Git</t>
+  </si>
+  <si>
+    <t>Create a repository that have all members as collaborators</t>
+  </si>
+  <si>
+    <t>Export to Binary</t>
+  </si>
+  <si>
+    <t>Export FBX file into a binary file format</t>
+  </si>
+  <si>
+    <t>Load and Render 2</t>
+  </si>
+  <si>
+    <t>Load and render from binary</t>
   </si>
 </sst>
 </file>
@@ -475,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1005"/>
+  <dimension ref="A1:AA1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -674,13 +680,13 @@
     </row>
     <row r="7" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -709,14 +715,15 @@
     </row>
     <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>5</v>
+      <c r="B8" s="9" t="s">
+        <v>13</v>
       </c>
-      <c r="C8" s="8">
-        <v>30</v>
+      <c r="C8" s="9">
+        <v>10</v>
       </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -743,15 +750,14 @@
     </row>
     <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="8">
         <v>10</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="9">
-        <v>30</v>
-      </c>
-      <c r="D9" s="1"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -776,17 +782,17 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>7</v>
+    <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>8</v>
+      <c r="B10" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="C10" s="9">
-        <v>25</v>
+        <v>30</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -811,17 +817,17 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C11" s="9">
-        <v>15</v>
+        <v>30</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -847,10 +853,16 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="9">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -875,11 +887,11 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -904,10 +916,10 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -934,10 +946,10 @@
       <c r="AA14" s="2"/>
     </row>
     <row r="15" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1050,7 +1062,7 @@
       <c r="AA18" s="2"/>
     </row>
     <row r="19" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1079,7 +1091,7 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
+      <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1165,8 +1177,8 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+    <row r="23" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1194,11 +1206,11 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
     </row>
-    <row r="24" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1224,10 +1236,10 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1253,10 +1265,10 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1398,7 +1410,7 @@
       <c r="AA30" s="2"/>
     </row>
     <row r="31" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
+      <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1427,7 +1439,7 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
+      <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1513,8 +1525,8 @@
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
+    <row r="35" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1542,11 +1554,11 @@
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
     </row>
-    <row r="36" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1572,10 +1584,10 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -1601,10 +1613,10 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -1746,7 +1758,7 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
+      <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1775,7 +1787,7 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
+      <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -29672,6 +29684,35 @@
       <c r="Z1005" s="2"/>
       <c r="AA1005" s="2"/>
     </row>
+    <row r="1006" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1006" s="2"/>
+      <c r="B1006" s="2"/>
+      <c r="C1006" s="2"/>
+      <c r="D1006" s="2"/>
+      <c r="E1006" s="2"/>
+      <c r="F1006" s="2"/>
+      <c r="G1006" s="2"/>
+      <c r="H1006" s="2"/>
+      <c r="I1006" s="2"/>
+      <c r="J1006" s="2"/>
+      <c r="K1006" s="2"/>
+      <c r="L1006" s="2"/>
+      <c r="M1006" s="2"/>
+      <c r="N1006" s="2"/>
+      <c r="O1006" s="2"/>
+      <c r="P1006" s="2"/>
+      <c r="Q1006" s="2"/>
+      <c r="R1006" s="2"/>
+      <c r="S1006" s="2"/>
+      <c r="T1006" s="2"/>
+      <c r="U1006" s="2"/>
+      <c r="V1006" s="2"/>
+      <c r="W1006" s="2"/>
+      <c r="X1006" s="2"/>
+      <c r="Y1006" s="2"/>
+      <c r="Z1006" s="2"/>
+      <c r="AA1006" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
updated milestone 1 excel
</commit_message>
<xml_diff>
--- a/GroupProject/SuperCoolFunYay Rubric.xlsx
+++ b/GroupProject/SuperCoolFunYay Rubric.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hedley\Desktop\RTA_SuperCoolFunYay\GroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01_SchoolWork\Programming\RTA\Project\RTA_SuperCoolFunYay\GroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,15 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>SuperCoolFunYay</t>
   </si>
   <si>
     <t>Katie Grinberg</t>
-  </si>
-  <si>
-    <t>Hedley Cayasso</t>
   </si>
   <si>
     <t>Milestone 1 Rubric</t>
@@ -56,25 +53,13 @@
     <t>Load and render from FBX</t>
   </si>
   <si>
-    <t>Setup base project with structures</t>
-  </si>
-  <si>
     <t>Setup Git</t>
   </si>
   <si>
     <t>Create a repository that have all members as collaborators</t>
   </si>
   <si>
-    <t>Export to Binary</t>
-  </si>
-  <si>
-    <t>Export FBX file into a binary file format</t>
-  </si>
-  <si>
-    <t>Load and Render 2</t>
-  </si>
-  <si>
-    <t>Load and render from binary</t>
+    <t>Setup base project with structures, get fbx api correctly attached</t>
   </si>
 </sst>
 </file>
@@ -481,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1006"/>
+  <dimension ref="A1:AA1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -559,7 +544,7 @@
     </row>
     <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -589,9 +574,7 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -619,9 +602,10 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
     </row>
-    <row r="5" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -648,11 +632,16 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>3</v>
+    <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>4</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="B6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -679,14 +668,14 @@
       <c r="AA6" s="2"/>
     </row>
     <row r="7" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>5</v>
+      <c r="A7" s="8" t="s">
+        <v>10</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>6</v>
+      <c r="B7" s="9" t="s">
+        <v>11</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>7</v>
+      <c r="C7" s="9">
+        <v>20</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -715,15 +704,14 @@
     </row>
     <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>13</v>
+      <c r="C8" s="8">
+        <v>30</v>
       </c>
-      <c r="C8" s="9">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -753,11 +741,12 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
-      <c r="C9" s="8">
-        <v>10</v>
+      <c r="C9" s="9">
+        <v>50</v>
       </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -783,16 +772,10 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="9">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -817,17 +800,11 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="9">
-        <v>30</v>
-      </c>
-      <c r="D11" s="5"/>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -853,15 +830,9 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="9">
-        <v>20</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -916,11 +887,11 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+    <row r="14" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -946,10 +917,10 @@
       <c r="AA14" s="2"/>
     </row>
     <row r="15" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1004,7 +975,7 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
+      <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1091,7 +1062,7 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1119,8 +1090,8 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
     </row>
-    <row r="21" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1149,10 +1120,10 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1178,10 +1149,10 @@
       <c r="AA22" s="2"/>
     </row>
     <row r="23" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1206,8 +1177,8 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+    <row r="24" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1236,10 +1207,10 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1265,10 +1236,10 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1352,7 +1323,7 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
+      <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1439,7 +1410,7 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
+      <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1467,8 +1438,8 @@
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
     </row>
-    <row r="33" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1497,10 +1468,10 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -1526,10 +1497,10 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -1554,8 +1525,8 @@
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
+    <row r="36" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1584,10 +1555,10 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -1613,10 +1584,10 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -1700,7 +1671,7 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
+      <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1787,7 +1758,7 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
+      <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -29626,93 +29597,6 @@
       <c r="Z1003" s="2"/>
       <c r="AA1003" s="2"/>
     </row>
-    <row r="1004" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1004" s="2"/>
-      <c r="B1004" s="2"/>
-      <c r="C1004" s="2"/>
-      <c r="D1004" s="2"/>
-      <c r="E1004" s="2"/>
-      <c r="F1004" s="2"/>
-      <c r="G1004" s="2"/>
-      <c r="H1004" s="2"/>
-      <c r="I1004" s="2"/>
-      <c r="J1004" s="2"/>
-      <c r="K1004" s="2"/>
-      <c r="L1004" s="2"/>
-      <c r="M1004" s="2"/>
-      <c r="N1004" s="2"/>
-      <c r="O1004" s="2"/>
-      <c r="P1004" s="2"/>
-      <c r="Q1004" s="2"/>
-      <c r="R1004" s="2"/>
-      <c r="S1004" s="2"/>
-      <c r="T1004" s="2"/>
-      <c r="U1004" s="2"/>
-      <c r="V1004" s="2"/>
-      <c r="W1004" s="2"/>
-      <c r="X1004" s="2"/>
-      <c r="Y1004" s="2"/>
-      <c r="Z1004" s="2"/>
-      <c r="AA1004" s="2"/>
-    </row>
-    <row r="1005" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1005" s="2"/>
-      <c r="B1005" s="2"/>
-      <c r="C1005" s="2"/>
-      <c r="D1005" s="2"/>
-      <c r="E1005" s="2"/>
-      <c r="F1005" s="2"/>
-      <c r="G1005" s="2"/>
-      <c r="H1005" s="2"/>
-      <c r="I1005" s="2"/>
-      <c r="J1005" s="2"/>
-      <c r="K1005" s="2"/>
-      <c r="L1005" s="2"/>
-      <c r="M1005" s="2"/>
-      <c r="N1005" s="2"/>
-      <c r="O1005" s="2"/>
-      <c r="P1005" s="2"/>
-      <c r="Q1005" s="2"/>
-      <c r="R1005" s="2"/>
-      <c r="S1005" s="2"/>
-      <c r="T1005" s="2"/>
-      <c r="U1005" s="2"/>
-      <c r="V1005" s="2"/>
-      <c r="W1005" s="2"/>
-      <c r="X1005" s="2"/>
-      <c r="Y1005" s="2"/>
-      <c r="Z1005" s="2"/>
-      <c r="AA1005" s="2"/>
-    </row>
-    <row r="1006" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1006" s="2"/>
-      <c r="B1006" s="2"/>
-      <c r="C1006" s="2"/>
-      <c r="D1006" s="2"/>
-      <c r="E1006" s="2"/>
-      <c r="F1006" s="2"/>
-      <c r="G1006" s="2"/>
-      <c r="H1006" s="2"/>
-      <c r="I1006" s="2"/>
-      <c r="J1006" s="2"/>
-      <c r="K1006" s="2"/>
-      <c r="L1006" s="2"/>
-      <c r="M1006" s="2"/>
-      <c r="N1006" s="2"/>
-      <c r="O1006" s="2"/>
-      <c r="P1006" s="2"/>
-      <c r="Q1006" s="2"/>
-      <c r="R1006" s="2"/>
-      <c r="S1006" s="2"/>
-      <c r="T1006" s="2"/>
-      <c r="U1006" s="2"/>
-      <c r="V1006" s="2"/>
-      <c r="W1006" s="2"/>
-      <c r="X1006" s="2"/>
-      <c r="Y1006" s="2"/>
-      <c r="Z1006" s="2"/>
-      <c r="AA1006" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>